<commit_message>
Integrate EU data for EoDfVUwFC, EoVPwFE, PTFURfE, SRPbVT
</commit_message>
<xml_diff>
--- a/InputData/trans/EoVPwFE/Elasticity of Veh Price wrt Fuel Econ.xlsx
+++ b/InputData/trans/EoVPwFE/Elasticity of Veh Price wrt Fuel Econ.xlsx
@@ -1,130 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\EoVPwFE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murielle.gagnebin\Documents\02_ProjetsPays\01_DE\2004_EPS_Europe\eps-us-2.1.0\InputData\trans\EoVPwFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F0D84F-017D-4584-BFE6-CB804B2F9324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="23955" windowHeight="13095"/>
+    <workbookView xWindow="7545" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Calculations" sheetId="2" r:id="rId2"/>
-    <sheet name="EoVPwFE" sheetId="3" r:id="rId3"/>
+    <sheet name="EoVPwFE" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Source:</t>
   </si>
   <si>
-    <t>Center for Automotive Research</t>
-  </si>
-  <si>
-    <t>The U.S. Automotive Market and Industry in 2025</t>
-  </si>
-  <si>
-    <t>http://www.cargroup.org/assets/files/ami.pdf</t>
-  </si>
-  <si>
-    <t>Page 24, Figure 9</t>
-  </si>
-  <si>
     <t>Incremental Cost for Fuel Economy</t>
   </si>
   <si>
-    <t>U.S. Environmental Protection Agency</t>
-  </si>
-  <si>
-    <t>EPA and NHTSA Set Standards to Reduce Greenhouse Gases and Improve Fuel Economy for Model Years 2017-2025 Cars and Light Trucks</t>
-  </si>
-  <si>
-    <t>http://www.epa.gov/otaq/climate/documents/420f12051.pdf</t>
-  </si>
-  <si>
-    <t>Page 2</t>
-  </si>
-  <si>
-    <t>Passenger LDV Base Cost</t>
-  </si>
-  <si>
-    <t>2016 Model Year MPG</t>
-  </si>
-  <si>
-    <t>2025 Model Year MPG</t>
-  </si>
-  <si>
-    <t>Incremental Cost (2016-2025)</t>
-  </si>
-  <si>
-    <t>Base LDV Cost</t>
-  </si>
-  <si>
-    <t>2016 Model Year Cost</t>
-  </si>
-  <si>
-    <t>2025 Model Year Cost</t>
-  </si>
-  <si>
-    <t>Assumes EPA value of $1800 is in real dollars</t>
-  </si>
-  <si>
-    <t>From U.S. EPA</t>
-  </si>
-  <si>
-    <t>% Improvement in Fuel Economy</t>
-  </si>
-  <si>
-    <t>% Increase in Price</t>
-  </si>
-  <si>
-    <t>Elasticity</t>
-  </si>
-  <si>
     <t>EoVPwFE Elasticity of Vehicle Price wrt Fuel Economy</t>
   </si>
   <si>
     <t>Vehicle Price wrt Fuel Econ</t>
   </si>
   <si>
-    <t>See "cpi.xlsx" in the InputData folder for source information.</t>
-  </si>
-  <si>
-    <t>The EPA and NHTSA document does not explicitly specify its curency year, and</t>
-  </si>
-  <si>
-    <t>it discusses costs in years 2017-2025, so we assume it is using currency of the year</t>
-  </si>
-  <si>
-    <t>of the document's publication, which is 2012.  Hence, no adjustment is needed.</t>
-  </si>
-  <si>
-    <t>The Center for Automotive Research's data was taken from a 2010 Automotive Yearbook</t>
-  </si>
-  <si>
-    <t>and therefore likely is in 2010 dollars.</t>
-  </si>
-  <si>
-    <t>We adjust 2010 dollars to 2012 dollars using the following conversion factor:</t>
-  </si>
-  <si>
-    <t>Currency Year</t>
-  </si>
-  <si>
-    <t>From Center for Automotive Research (2010$)</t>
-  </si>
-  <si>
-    <t>In 2012$ dollars</t>
-  </si>
-  <si>
     <t>The model uses LDVs elasticity for all vehicle types because no data on price elasticity</t>
   </si>
   <si>
@@ -132,24 +50,64 @@
   </si>
   <si>
     <t>Elasticity (dimensionless)</t>
+  </si>
+  <si>
+    <t>https://www.iea.org/reports/fuel-economy-in-major-car-markets</t>
+  </si>
+  <si>
+    <t>https://advocacy.consumerreports.org/research/more-mileage-for-your-money-report/</t>
+  </si>
+  <si>
+    <t>http://energyfuse.org/how-much-have-fuel-economy-standards-boosted-the-price-of-cars/</t>
+  </si>
+  <si>
+    <t>Several articles and reports state that fuel economy has been improving but</t>
+  </si>
+  <si>
+    <t>average new vehicle price has been stagnating, in real terms even slightly decreasing</t>
+  </si>
+  <si>
+    <t>in the past years depending on the region.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The IEA report mentions "When looking at vehicles in the same market segment, </t>
+  </si>
+  <si>
+    <t>with similar power and size, and with the same powertrain type, fuel efficiency</t>
+  </si>
+  <si>
+    <t>is not coupled with higher vehicle prices. The 25% most efficient vehicles cost</t>
+  </si>
+  <si>
+    <t>5-7% less than the average equivalent vehicle, and the average fuel economy</t>
+  </si>
+  <si>
+    <t>IEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuel Economy in Major Car Markets - Technology and Policy Drivers 2005-2017 </t>
+  </si>
+  <si>
+    <t>improvements they deliver are 0.6 Lge/100 km." (for an average fuel economy</t>
+  </si>
+  <si>
+    <t>of 5.6 Lge/100km for LDVs in 2017 in the 26 European countries investigated).</t>
+  </si>
+  <si>
+    <t>Page 48-49</t>
+  </si>
+  <si>
+    <t>So the elasticity is set to 0 for Europe.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,58 +214,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Body: normal cell" xfId="6"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="4"/>
-    <cellStyle name="Footnotes: top row" xfId="8"/>
-    <cellStyle name="Header: bottom row" xfId="5"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="7"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Table title" xfId="3"/>
+  <cellStyles count="8">
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -323,7 +275,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -398,6 +350,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -433,6 +402,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -608,14 +594,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD23"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="57.5703125" customWidth="1"/>
@@ -623,7 +609,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -631,126 +617,158 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
-        <v>2012</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="11" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="13" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-    </row>
-    <row r="21" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>1.0549999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>24</v>
-      </c>
+    <row r="17" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1"/>
-    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{5A72898E-2BB5-44B1-A32B-0479598ADC60}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{62EDE884-5AE9-4D9C-8874-0C0FB8E88859}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -758,150 +776,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1">
-        <v>35.5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>54.5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1800</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="5">
-        <v>23186</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="5">
-        <f>B4*About!A27</f>
-        <v>24461.23</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="5">
-        <f>B5+B3</f>
-        <v>26261.23</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="6">
-        <f>(B2-B1)/B1</f>
-        <v>0.53521126760563376</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="6">
-        <f>(B6-B5)/B5</f>
-        <v>7.358583358236688E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="7">
-        <f>B9/B8</f>
-        <v>0.13748932064073813</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
-        <v>36</v>
+      <c r="B1" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="8">
-        <f>Calculations!B11</f>
-        <v>0.13748932064073813</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>